<commit_message>
add write to sql file
</commit_message>
<xml_diff>
--- a/src/main/resources/upload-dir/staffList_2024_10.xlsx
+++ b/src/main/resources/upload-dir/staffList_2024_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Поточна робота\Премії\премія файли\премія_листопад\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35668CCD-F863-4970-A0AE-BB0BFD582C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48C11E4-0418-4EE8-A455-77C06D37AF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11494,11 +11494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:X1197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22780,7 +22779,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="161" spans="1:24" hidden="1">
+    <row r="161" spans="1:24">
       <c r="A161" s="4">
         <v>165</v>
       </c>
@@ -22924,7 +22923,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="163" spans="1:24" hidden="1">
+    <row r="163" spans="1:24">
       <c r="A163" s="4">
         <v>167</v>
       </c>
@@ -23284,7 +23283,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="168" spans="1:24" hidden="1">
+    <row r="168" spans="1:24">
       <c r="A168" s="4">
         <v>172</v>
       </c>
@@ -49420,7 +49419,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="531" spans="1:24" hidden="1">
+    <row r="531" spans="1:24">
       <c r="A531" s="4">
         <v>535</v>
       </c>
@@ -49492,7 +49491,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="532" spans="1:24" hidden="1">
+    <row r="532" spans="1:24">
       <c r="A532" s="4">
         <v>536</v>
       </c>
@@ -49564,7 +49563,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="533" spans="1:24" hidden="1">
+    <row r="533" spans="1:24">
       <c r="A533" s="4">
         <v>537</v>
       </c>
@@ -49636,7 +49635,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="534" spans="1:24" hidden="1">
+    <row r="534" spans="1:24">
       <c r="A534" s="4">
         <v>538</v>
       </c>
@@ -49708,7 +49707,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="535" spans="1:24" hidden="1">
+    <row r="535" spans="1:24">
       <c r="A535" s="4">
         <v>539</v>
       </c>
@@ -58060,7 +58059,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="651" spans="1:24" hidden="1">
+    <row r="651" spans="1:24">
       <c r="A651" s="4">
         <v>655</v>
       </c>
@@ -58132,7 +58131,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="652" spans="1:24" hidden="1">
+    <row r="652" spans="1:24">
       <c r="A652" s="4">
         <v>656</v>
       </c>
@@ -58204,7 +58203,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="653" spans="1:24" hidden="1">
+    <row r="653" spans="1:24">
       <c r="A653" s="4">
         <v>657</v>
       </c>
@@ -58276,7 +58275,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="654" spans="1:24" hidden="1">
+    <row r="654" spans="1:24">
       <c r="A654" s="4">
         <v>658</v>
       </c>
@@ -58348,7 +58347,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="655" spans="1:24" hidden="1">
+    <row r="655" spans="1:24">
       <c r="A655" s="4">
         <v>659</v>
       </c>
@@ -58420,7 +58419,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="656" spans="1:24" hidden="1">
+    <row r="656" spans="1:24">
       <c r="A656" s="4">
         <v>660</v>
       </c>
@@ -60580,7 +60579,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="686" spans="1:24" hidden="1">
+    <row r="686" spans="1:24">
       <c r="A686" s="4">
         <v>690</v>
       </c>
@@ -60652,7 +60651,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="687" spans="1:24" hidden="1">
+    <row r="687" spans="1:24">
       <c r="A687" s="4">
         <v>691</v>
       </c>
@@ -60724,7 +60723,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="688" spans="1:24" hidden="1">
+    <row r="688" spans="1:24">
       <c r="A688" s="4">
         <v>692</v>
       </c>
@@ -60796,7 +60795,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="689" spans="1:24" hidden="1">
+    <row r="689" spans="1:24">
       <c r="A689" s="4">
         <v>693</v>
       </c>
@@ -60868,7 +60867,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="690" spans="1:24" hidden="1">
+    <row r="690" spans="1:24">
       <c r="A690" s="4">
         <v>694</v>
       </c>
@@ -60940,7 +60939,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="691" spans="1:24" hidden="1">
+    <row r="691" spans="1:24">
       <c r="A691" s="4">
         <v>695</v>
       </c>
@@ -61012,7 +61011,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="692" spans="1:24" hidden="1">
+    <row r="692" spans="1:24">
       <c r="A692" s="4">
         <v>696</v>
       </c>
@@ -61084,7 +61083,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="693" spans="1:24" hidden="1">
+    <row r="693" spans="1:24">
       <c r="A693" s="4">
         <v>697</v>
       </c>
@@ -61300,7 +61299,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="696" spans="1:24" hidden="1">
+    <row r="696" spans="1:24">
       <c r="A696" s="4">
         <v>700</v>
       </c>
@@ -61372,7 +61371,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="697" spans="1:24" hidden="1">
+    <row r="697" spans="1:24">
       <c r="A697" s="4">
         <v>701</v>
       </c>
@@ -61444,7 +61443,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="698" spans="1:24" hidden="1">
+    <row r="698" spans="1:24">
       <c r="A698" s="4">
         <v>702</v>
       </c>
@@ -84412,7 +84411,7 @@
         <v>3681</v>
       </c>
     </row>
-    <row r="1017" spans="1:24" hidden="1">
+    <row r="1017" spans="1:24">
       <c r="A1017" s="4">
         <v>1021</v>
       </c>
@@ -84484,7 +84483,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1018" spans="1:24" hidden="1">
+    <row r="1018" spans="1:24">
       <c r="A1018" s="4">
         <v>1022</v>
       </c>
@@ -84556,7 +84555,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1019" spans="1:24" hidden="1">
+    <row r="1019" spans="1:24">
       <c r="A1019" s="4">
         <v>1023</v>
       </c>
@@ -84628,7 +84627,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1020" spans="1:24" hidden="1">
+    <row r="1020" spans="1:24">
       <c r="A1020" s="4">
         <v>1024</v>
       </c>
@@ -84700,7 +84699,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1021" spans="1:24" hidden="1">
+    <row r="1021" spans="1:24">
       <c r="A1021" s="4">
         <v>1025</v>
       </c>
@@ -84772,7 +84771,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1022" spans="1:24" hidden="1">
+    <row r="1022" spans="1:24">
       <c r="A1022" s="4">
         <v>1026</v>
       </c>
@@ -84844,7 +84843,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1023" spans="1:24" hidden="1">
+    <row r="1023" spans="1:24">
       <c r="A1023" s="4">
         <v>1027</v>
       </c>
@@ -84916,7 +84915,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1024" spans="1:24" hidden="1">
+    <row r="1024" spans="1:24">
       <c r="A1024" s="4">
         <v>1028</v>
       </c>
@@ -84988,7 +84987,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1025" spans="1:24" hidden="1">
+    <row r="1025" spans="1:24">
       <c r="A1025" s="4">
         <v>1029</v>
       </c>
@@ -85060,7 +85059,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1026" spans="1:24" hidden="1">
+    <row r="1026" spans="1:24">
       <c r="A1026" s="4">
         <v>1030</v>
       </c>
@@ -85132,7 +85131,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1027" spans="1:24" hidden="1">
+    <row r="1027" spans="1:24">
       <c r="A1027" s="4">
         <v>1031</v>
       </c>
@@ -85204,7 +85203,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1028" spans="1:24" hidden="1">
+    <row r="1028" spans="1:24">
       <c r="A1028" s="4">
         <v>1032</v>
       </c>
@@ -85276,7 +85275,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1029" spans="1:24" hidden="1">
+    <row r="1029" spans="1:24">
       <c r="A1029" s="4">
         <v>1033</v>
       </c>
@@ -85348,7 +85347,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1030" spans="1:24" hidden="1">
+    <row r="1030" spans="1:24">
       <c r="A1030" s="4">
         <v>1034</v>
       </c>
@@ -85420,7 +85419,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1031" spans="1:24" hidden="1">
+    <row r="1031" spans="1:24">
       <c r="A1031" s="4">
         <v>1035</v>
       </c>
@@ -85492,7 +85491,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="1032" spans="1:24" hidden="1">
+    <row r="1032" spans="1:24">
       <c r="A1032" s="4">
         <v>1036</v>
       </c>
@@ -97450,11 +97449,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:X1197" xr:uid="{EFB53C6D-1575-4582-816D-BC2B6A26BB91}">
-    <filterColumn colId="23">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:X1197" xr:uid="{EFB53C6D-1575-4582-816D-BC2B6A26BB91}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>